<commit_message>
Agregado lista de precios marzo
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecilia y Lucas\Dropbox\LUCAS PICONE OMINT\2025 OMINT OK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecilia y Lucas\Dropbox\LUCAS PICONE OMINT\2025 OMINT OK\COTIZADOR\COTIZADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,10 +81,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,11 +100,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Antique Olive"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -114,19 +110,20 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -153,25 +150,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,12 +454,13 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
@@ -467,7 +469,7 @@
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,294 +495,264 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
-        <f>C2-C2*30%</f>
-        <v>85439.200000000012</v>
-      </c>
-      <c r="C2" s="3">
-        <v>122056</v>
-      </c>
-      <c r="D2" s="3">
-        <v>144121</v>
-      </c>
-      <c r="E2" s="3">
-        <v>244327</v>
-      </c>
-      <c r="F2" s="3">
-        <v>366168</v>
-      </c>
-      <c r="G2" s="3">
-        <f>C2-C2*40%</f>
-        <v>73233.600000000006</v>
-      </c>
-      <c r="H2" s="3">
-        <f>C2-C2*50%</f>
-        <v>61028</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="3">
+        <v>87138</v>
+      </c>
+      <c r="C2" s="4">
+        <v>124741</v>
+      </c>
+      <c r="D2" s="4">
+        <v>147292</v>
+      </c>
+      <c r="E2" s="4">
+        <v>249702</v>
+      </c>
+      <c r="F2" s="4">
+        <v>387946</v>
+      </c>
+      <c r="G2" s="4">
+        <v>75893</v>
+      </c>
+      <c r="H2" s="4">
+        <v>65463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ref="B3:B6" si="0">C3-C3*30%</f>
-        <v>86753.1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>123933</v>
-      </c>
-      <c r="D3" s="3">
-        <v>145485</v>
-      </c>
-      <c r="E3" s="3">
-        <v>251054</v>
-      </c>
-      <c r="F3" s="3">
-        <v>371799</v>
-      </c>
-      <c r="G3" s="3">
-        <f>C3-C3*40%</f>
-        <v>74359.799999999988</v>
-      </c>
-      <c r="H3" s="3">
-        <f>C3-C3*50%</f>
-        <v>61966.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="4">
+        <v>87519</v>
+      </c>
+      <c r="C3" s="4">
+        <v>126660</v>
+      </c>
+      <c r="D3" s="4">
+        <v>148686</v>
+      </c>
+      <c r="E3" s="4">
+        <v>256577</v>
+      </c>
+      <c r="F3" s="4">
+        <v>389147</v>
+      </c>
+      <c r="G3" s="4">
+        <v>76091</v>
+      </c>
+      <c r="H3" s="4">
+        <v>65721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" si="0"/>
-        <v>97797</v>
-      </c>
-      <c r="C4" s="3">
-        <v>139710</v>
-      </c>
-      <c r="D4" s="3">
-        <v>163934</v>
-      </c>
-      <c r="E4" s="3">
-        <v>282575</v>
-      </c>
-      <c r="F4" s="3">
-        <v>419130</v>
-      </c>
-      <c r="G4" s="3">
-        <f>C4-C4*40%</f>
-        <v>83826</v>
-      </c>
-      <c r="H4" s="3">
-        <f>C4-C4*50%</f>
-        <v>69855</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="4">
+        <v>98448</v>
+      </c>
+      <c r="C4" s="4">
+        <v>142784</v>
+      </c>
+      <c r="D4" s="4">
+        <v>167541</v>
+      </c>
+      <c r="E4" s="4">
+        <v>288792</v>
+      </c>
+      <c r="F4" s="4">
+        <v>438165</v>
+      </c>
+      <c r="G4" s="4">
+        <v>85509</v>
+      </c>
+      <c r="H4" s="4">
+        <v>74130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" si="0"/>
-        <v>122481.8</v>
-      </c>
-      <c r="C5" s="3">
-        <v>174974</v>
-      </c>
-      <c r="D5" s="3">
-        <v>204948</v>
-      </c>
-      <c r="E5" s="3">
-        <v>343443</v>
-      </c>
-      <c r="F5" s="3">
-        <v>524922</v>
-      </c>
-      <c r="G5" s="3">
-        <f>C5-C5*40%</f>
-        <v>104984.4</v>
-      </c>
-      <c r="H5" s="3">
-        <f>C5-C5*50%</f>
-        <v>87487</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="4">
+        <v>125067</v>
+      </c>
+      <c r="C5" s="4">
+        <v>178823</v>
+      </c>
+      <c r="D5" s="4">
+        <v>209457</v>
+      </c>
+      <c r="E5" s="4">
+        <v>350999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>522638</v>
+      </c>
+      <c r="G5" s="4">
+        <v>109102</v>
+      </c>
+      <c r="H5" s="4">
+        <v>94896</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" si="0"/>
-        <v>196200.90000000002</v>
-      </c>
-      <c r="C6" s="3">
-        <v>280287</v>
-      </c>
-      <c r="D6" s="3">
-        <v>368903</v>
-      </c>
-      <c r="E6" s="3">
-        <v>514184</v>
-      </c>
-      <c r="F6" s="3">
-        <v>840861</v>
-      </c>
-      <c r="G6" s="3">
-        <f>C6-C6*40%</f>
-        <v>168172.2</v>
-      </c>
-      <c r="H6" s="3">
-        <f>C6-C6*50%</f>
-        <v>140143.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="4">
+        <v>215047</v>
+      </c>
+      <c r="C6" s="4">
+        <v>286453</v>
+      </c>
+      <c r="D6" s="4">
+        <v>377019</v>
+      </c>
+      <c r="E6" s="4">
+        <v>525496</v>
+      </c>
+      <c r="F6" s="4">
+        <v>716108</v>
+      </c>
+      <c r="G6" s="4">
+        <v>188431</v>
+      </c>
+      <c r="H6" s="4">
+        <v>164452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2">
-        <f>C7-C7*30%</f>
-        <v>55518.400000000001</v>
-      </c>
-      <c r="C7" s="3">
-        <v>79312</v>
-      </c>
-      <c r="D7" s="3">
-        <v>98479</v>
-      </c>
-      <c r="E7" s="3">
-        <v>186135</v>
-      </c>
-      <c r="F7" s="3">
-        <v>237936</v>
-      </c>
-      <c r="G7" s="3">
-        <f>C7-C7*35%</f>
-        <v>51552.800000000003</v>
-      </c>
-      <c r="H7" s="3">
-        <f>C7-C7*40%</f>
-        <v>47587.199999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="4">
+        <v>56239</v>
+      </c>
+      <c r="C7" s="4">
+        <v>81057</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100646</v>
+      </c>
+      <c r="E7" s="4">
+        <v>190230</v>
+      </c>
+      <c r="F7" s="4">
+        <v>277538</v>
+      </c>
+      <c r="G7" s="4">
+        <v>53461</v>
+      </c>
+      <c r="H7" s="4">
+        <v>48114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" ref="B8:B10" si="1">C8-C8*30%</f>
-        <v>56065.8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>80094</v>
-      </c>
-      <c r="D8" s="3">
-        <v>98446</v>
-      </c>
-      <c r="E8" s="3">
-        <v>187667</v>
-      </c>
-      <c r="F8" s="3">
-        <v>240282</v>
-      </c>
-      <c r="G8" s="3">
-        <f>C8-C8*35%</f>
-        <v>52061.100000000006</v>
-      </c>
-      <c r="H8" s="3">
-        <f>C8-C8*40%</f>
-        <v>48056.399999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="4">
+        <v>57295</v>
+      </c>
+      <c r="C8" s="4">
+        <v>81856</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100612</v>
+      </c>
+      <c r="E8" s="4">
+        <v>191796</v>
+      </c>
+      <c r="F8" s="4">
+        <v>282690</v>
+      </c>
+      <c r="G8" s="4">
+        <v>53205</v>
+      </c>
+      <c r="H8" s="4">
+        <v>49658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" si="1"/>
-        <v>63465.5</v>
-      </c>
-      <c r="C9" s="3">
-        <v>90665</v>
-      </c>
-      <c r="D9" s="3">
-        <v>113665</v>
-      </c>
-      <c r="E9" s="3">
-        <v>217742</v>
-      </c>
-      <c r="F9" s="3">
-        <v>271995</v>
-      </c>
-      <c r="G9" s="3">
-        <f>C9-C9*35%</f>
-        <v>58932.25</v>
-      </c>
-      <c r="H9" s="3">
-        <f>C9-C9*40%</f>
-        <v>54399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="4">
+        <v>65759</v>
+      </c>
+      <c r="C9" s="4">
+        <v>92660</v>
+      </c>
+      <c r="D9" s="4">
+        <v>116166</v>
+      </c>
+      <c r="E9" s="4">
+        <v>222532</v>
+      </c>
+      <c r="F9" s="4">
+        <v>326411</v>
+      </c>
+      <c r="G9" s="4">
+        <v>62203</v>
+      </c>
+      <c r="H9" s="4">
+        <v>58266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
-        <f t="shared" si="1"/>
-        <v>77164.5</v>
-      </c>
-      <c r="C10" s="3">
-        <v>110235</v>
-      </c>
-      <c r="D10" s="3">
-        <v>135386</v>
-      </c>
-      <c r="E10" s="3">
-        <v>262148</v>
-      </c>
-      <c r="F10" s="3">
-        <v>330705</v>
-      </c>
-      <c r="G10" s="3">
-        <f>C10-C10*35%</f>
-        <v>71652.75</v>
-      </c>
-      <c r="H10" s="3">
-        <f>C10-C10*40%</f>
-        <v>66141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="4">
+        <v>80143</v>
+      </c>
+      <c r="C10" s="4">
+        <v>112660</v>
+      </c>
+      <c r="D10" s="4">
+        <v>138364</v>
+      </c>
+      <c r="E10" s="4">
+        <v>267915</v>
+      </c>
+      <c r="F10" s="4">
+        <v>381955</v>
+      </c>
+      <c r="G10" s="4">
+        <v>74729</v>
+      </c>
+      <c r="H10" s="4">
+        <v>69999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2">
-        <f>C11-C11*30%</f>
-        <v>72622.899999999994</v>
-      </c>
-      <c r="C11" s="3">
-        <v>103747</v>
-      </c>
-      <c r="D11" s="3">
-        <v>122502</v>
-      </c>
-      <c r="E11" s="3">
-        <v>207678</v>
-      </c>
-      <c r="F11" s="3">
-        <v>311241</v>
-      </c>
-      <c r="G11" s="3">
-        <f>C11-C11*40%</f>
-        <v>62248.2</v>
-      </c>
-      <c r="H11" s="3">
-        <f>C11-C11*50%</f>
-        <v>51873.5</v>
+      <c r="B11" s="4">
+        <v>74066</v>
+      </c>
+      <c r="C11" s="4">
+        <v>106029</v>
+      </c>
+      <c r="D11" s="4">
+        <v>125197</v>
+      </c>
+      <c r="E11" s="4">
+        <v>212247</v>
+      </c>
+      <c r="F11" s="4">
+        <v>329753</v>
+      </c>
+      <c r="G11" s="4">
+        <v>64509</v>
+      </c>
+      <c r="H11" s="4">
+        <v>55644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar listas de precios en cotizador.xlsx
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -81,8 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -150,12 +149,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,16 +161,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
-    <cellStyle name="Moneda 2" xfId="2"/>
+  <cellStyles count="2">
+    <cellStyle name="Moneda 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,7 +448,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,259 +494,259 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>87138</v>
-      </c>
-      <c r="C2" s="4">
-        <v>124741</v>
-      </c>
-      <c r="D2" s="4">
-        <v>147292</v>
-      </c>
-      <c r="E2" s="4">
-        <v>249702</v>
-      </c>
-      <c r="F2" s="4">
-        <v>387946</v>
-      </c>
-      <c r="G2" s="4">
-        <v>75893</v>
-      </c>
-      <c r="H2" s="4">
-        <v>65463</v>
+        <v>89229</v>
+      </c>
+      <c r="C2" s="3">
+        <v>127735</v>
+      </c>
+      <c r="D2" s="3">
+        <v>150827</v>
+      </c>
+      <c r="E2" s="3">
+        <v>255695</v>
+      </c>
+      <c r="F2" s="3">
+        <v>397257</v>
+      </c>
+      <c r="G2" s="3">
+        <v>77714</v>
+      </c>
+      <c r="H2" s="3">
+        <v>67034</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
-        <v>87519</v>
-      </c>
-      <c r="C3" s="4">
-        <v>126660</v>
-      </c>
-      <c r="D3" s="4">
-        <v>148686</v>
-      </c>
-      <c r="E3" s="4">
-        <v>256577</v>
-      </c>
-      <c r="F3" s="4">
-        <v>389147</v>
-      </c>
-      <c r="G3" s="4">
-        <v>76091</v>
-      </c>
-      <c r="H3" s="4">
-        <v>65721</v>
+      <c r="B3" s="3">
+        <v>89619</v>
+      </c>
+      <c r="C3" s="3">
+        <v>129700</v>
+      </c>
+      <c r="D3" s="3">
+        <v>152254</v>
+      </c>
+      <c r="E3" s="3">
+        <v>262735</v>
+      </c>
+      <c r="F3" s="3">
+        <v>398487</v>
+      </c>
+      <c r="G3" s="3">
+        <v>77917</v>
+      </c>
+      <c r="H3" s="3">
+        <v>67298</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
-        <v>98448</v>
-      </c>
-      <c r="C4" s="4">
-        <v>142784</v>
-      </c>
-      <c r="D4" s="4">
-        <v>167541</v>
-      </c>
-      <c r="E4" s="4">
-        <v>288792</v>
-      </c>
-      <c r="F4" s="4">
-        <v>438165</v>
-      </c>
-      <c r="G4" s="4">
-        <v>85509</v>
-      </c>
-      <c r="H4" s="4">
-        <v>74130</v>
+      <c r="B4" s="3">
+        <v>100811</v>
+      </c>
+      <c r="C4" s="3">
+        <v>146211</v>
+      </c>
+      <c r="D4" s="3">
+        <v>171562</v>
+      </c>
+      <c r="E4" s="3">
+        <v>295723</v>
+      </c>
+      <c r="F4" s="3">
+        <v>448681</v>
+      </c>
+      <c r="G4" s="3">
+        <v>87561</v>
+      </c>
+      <c r="H4" s="3">
+        <v>75909</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
-        <v>125067</v>
-      </c>
-      <c r="C5" s="4">
-        <v>178823</v>
-      </c>
-      <c r="D5" s="4">
-        <v>209457</v>
-      </c>
-      <c r="E5" s="4">
-        <v>350999</v>
-      </c>
-      <c r="F5" s="4">
-        <v>522638</v>
-      </c>
-      <c r="G5" s="4">
-        <v>109102</v>
-      </c>
-      <c r="H5" s="4">
-        <v>94896</v>
+      <c r="B5" s="3">
+        <v>128069</v>
+      </c>
+      <c r="C5" s="3">
+        <v>183115</v>
+      </c>
+      <c r="D5" s="3">
+        <v>214484</v>
+      </c>
+      <c r="E5" s="3">
+        <v>359423</v>
+      </c>
+      <c r="F5" s="3">
+        <v>535181</v>
+      </c>
+      <c r="G5" s="3">
+        <v>111720</v>
+      </c>
+      <c r="H5" s="3">
+        <v>97174</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
-        <v>215047</v>
-      </c>
-      <c r="C6" s="4">
-        <v>286453</v>
-      </c>
-      <c r="D6" s="4">
-        <v>377019</v>
-      </c>
-      <c r="E6" s="4">
-        <v>525496</v>
-      </c>
-      <c r="F6" s="4">
-        <v>716108</v>
-      </c>
-      <c r="G6" s="4">
-        <v>188431</v>
-      </c>
-      <c r="H6" s="4">
-        <v>164452</v>
+      <c r="B6" s="3">
+        <v>220208</v>
+      </c>
+      <c r="C6" s="3">
+        <v>293328</v>
+      </c>
+      <c r="D6" s="3">
+        <v>386067</v>
+      </c>
+      <c r="E6" s="3">
+        <v>538108</v>
+      </c>
+      <c r="F6" s="3">
+        <v>733295</v>
+      </c>
+      <c r="G6" s="3">
+        <v>192953</v>
+      </c>
+      <c r="H6" s="3">
+        <v>168399</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4">
-        <v>56239</v>
-      </c>
-      <c r="C7" s="4">
-        <v>81057</v>
-      </c>
-      <c r="D7" s="4">
-        <v>100646</v>
-      </c>
-      <c r="E7" s="4">
-        <v>190230</v>
-      </c>
-      <c r="F7" s="4">
-        <v>277538</v>
-      </c>
-      <c r="G7" s="4">
-        <v>53461</v>
-      </c>
-      <c r="H7" s="4">
-        <v>48114</v>
+      <c r="B7" s="3">
+        <v>57589</v>
+      </c>
+      <c r="C7" s="3">
+        <v>83002</v>
+      </c>
+      <c r="D7" s="3">
+        <v>103062</v>
+      </c>
+      <c r="E7" s="3">
+        <v>194796</v>
+      </c>
+      <c r="F7" s="3">
+        <v>284199</v>
+      </c>
+      <c r="G7" s="3">
+        <v>54744</v>
+      </c>
+      <c r="H7" s="3">
+        <v>49269</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4">
-        <v>57295</v>
-      </c>
-      <c r="C8" s="4">
-        <v>81856</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100612</v>
-      </c>
-      <c r="E8" s="4">
-        <v>191796</v>
-      </c>
-      <c r="F8" s="4">
-        <v>282690</v>
-      </c>
-      <c r="G8" s="4">
-        <v>53205</v>
-      </c>
-      <c r="H8" s="4">
-        <v>49658</v>
+      <c r="B8" s="3">
+        <v>58670</v>
+      </c>
+      <c r="C8" s="3">
+        <v>83821</v>
+      </c>
+      <c r="D8" s="3">
+        <v>103027</v>
+      </c>
+      <c r="E8" s="3">
+        <v>196399</v>
+      </c>
+      <c r="F8" s="3">
+        <v>289475</v>
+      </c>
+      <c r="G8" s="3">
+        <v>54482</v>
+      </c>
+      <c r="H8" s="3">
+        <v>50850</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4">
-        <v>65759</v>
-      </c>
-      <c r="C9" s="4">
-        <v>92660</v>
-      </c>
-      <c r="D9" s="4">
-        <v>116166</v>
-      </c>
-      <c r="E9" s="4">
-        <v>222532</v>
-      </c>
-      <c r="F9" s="4">
-        <v>326411</v>
-      </c>
-      <c r="G9" s="4">
-        <v>62203</v>
-      </c>
-      <c r="H9" s="4">
-        <v>58266</v>
+      <c r="B9" s="3">
+        <v>67337</v>
+      </c>
+      <c r="C9" s="3">
+        <v>94884</v>
+      </c>
+      <c r="D9" s="3">
+        <v>118954</v>
+      </c>
+      <c r="E9" s="3">
+        <v>227873</v>
+      </c>
+      <c r="F9" s="3">
+        <v>334245</v>
+      </c>
+      <c r="G9" s="3">
+        <v>63696</v>
+      </c>
+      <c r="H9" s="3">
+        <v>59664</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4">
-        <v>80143</v>
-      </c>
-      <c r="C10" s="4">
-        <v>112660</v>
-      </c>
-      <c r="D10" s="4">
-        <v>138364</v>
-      </c>
-      <c r="E10" s="4">
-        <v>267915</v>
-      </c>
-      <c r="F10" s="4">
-        <v>381955</v>
-      </c>
-      <c r="G10" s="4">
-        <v>74729</v>
-      </c>
-      <c r="H10" s="4">
-        <v>69999</v>
+      <c r="B10" s="3">
+        <v>82066</v>
+      </c>
+      <c r="C10" s="3">
+        <v>115364</v>
+      </c>
+      <c r="D10" s="3">
+        <v>141685</v>
+      </c>
+      <c r="E10" s="3">
+        <v>274345</v>
+      </c>
+      <c r="F10" s="3">
+        <v>391122</v>
+      </c>
+      <c r="G10" s="3">
+        <v>76522</v>
+      </c>
+      <c r="H10" s="3">
+        <v>71679</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4">
-        <v>74066</v>
-      </c>
-      <c r="C11" s="4">
-        <v>106029</v>
-      </c>
-      <c r="D11" s="4">
-        <v>125197</v>
-      </c>
-      <c r="E11" s="4">
-        <v>212247</v>
-      </c>
-      <c r="F11" s="4">
-        <v>329753</v>
-      </c>
-      <c r="G11" s="4">
-        <v>64509</v>
-      </c>
-      <c r="H11" s="4">
-        <v>55644</v>
+      <c r="B11" s="3">
+        <v>75844</v>
+      </c>
+      <c r="C11" s="3">
+        <v>108574</v>
+      </c>
+      <c r="D11" s="3">
+        <v>128202</v>
+      </c>
+      <c r="E11" s="3">
+        <v>217341</v>
+      </c>
+      <c r="F11" s="3">
+        <v>337667</v>
+      </c>
+      <c r="G11" s="3">
+        <v>66057</v>
+      </c>
+      <c r="H11" s="3">
+        <v>56979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar listas de precios - mayo
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -161,7 +161,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -448,7 +448,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,25 +494,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>89229</v>
+        <v>92263</v>
       </c>
       <c r="C2" s="3">
-        <v>127735</v>
+        <v>132078</v>
       </c>
       <c r="D2" s="3">
-        <v>150827</v>
+        <v>155955</v>
       </c>
       <c r="E2" s="3">
-        <v>255695</v>
+        <v>264389</v>
       </c>
       <c r="F2" s="3">
-        <v>397257</v>
+        <v>410764</v>
       </c>
       <c r="G2" s="3">
-        <v>77714</v>
+        <v>80356</v>
       </c>
       <c r="H2" s="3">
-        <v>67034</v>
+        <v>69313</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -520,25 +520,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>89619</v>
+        <v>92666</v>
       </c>
       <c r="C3" s="3">
-        <v>129700</v>
+        <v>134110</v>
       </c>
       <c r="D3" s="3">
-        <v>152254</v>
+        <v>157431</v>
       </c>
       <c r="E3" s="3">
-        <v>262735</v>
+        <v>271668</v>
       </c>
       <c r="F3" s="3">
-        <v>398487</v>
+        <v>412036</v>
       </c>
       <c r="G3" s="3">
-        <v>77917</v>
+        <v>80566</v>
       </c>
       <c r="H3" s="3">
-        <v>67298</v>
+        <v>69586</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -546,25 +546,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>100811</v>
+        <v>104239</v>
       </c>
       <c r="C4" s="3">
-        <v>146211</v>
+        <v>151182</v>
       </c>
       <c r="D4" s="3">
-        <v>171562</v>
+        <v>177395</v>
       </c>
       <c r="E4" s="3">
-        <v>295723</v>
+        <v>305778</v>
       </c>
       <c r="F4" s="3">
-        <v>448681</v>
+        <v>463936</v>
       </c>
       <c r="G4" s="3">
-        <v>87561</v>
+        <v>90538</v>
       </c>
       <c r="H4" s="3">
-        <v>75909</v>
+        <v>78490</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -572,25 +572,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>128069</v>
+        <v>132423</v>
       </c>
       <c r="C5" s="3">
-        <v>183115</v>
+        <v>189341</v>
       </c>
       <c r="D5" s="3">
-        <v>214484</v>
+        <v>221776</v>
       </c>
       <c r="E5" s="3">
-        <v>359423</v>
+        <v>371643</v>
       </c>
       <c r="F5" s="3">
-        <v>535181</v>
+        <v>553377</v>
       </c>
       <c r="G5" s="3">
-        <v>111720</v>
+        <v>115518</v>
       </c>
       <c r="H5" s="3">
-        <v>97174</v>
+        <v>100478</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -598,25 +598,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>220208</v>
+        <v>227695</v>
       </c>
       <c r="C6" s="3">
-        <v>293328</v>
+        <v>303301</v>
       </c>
       <c r="D6" s="3">
-        <v>386067</v>
+        <v>399193</v>
       </c>
       <c r="E6" s="3">
-        <v>538108</v>
+        <v>556404</v>
       </c>
       <c r="F6" s="3">
-        <v>733295</v>
+        <v>758227</v>
       </c>
       <c r="G6" s="3">
-        <v>192953</v>
+        <v>199513</v>
       </c>
       <c r="H6" s="3">
-        <v>168399</v>
+        <v>174125</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -624,25 +624,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>57589</v>
+        <v>59547</v>
       </c>
       <c r="C7" s="3">
-        <v>83002</v>
+        <v>85824</v>
       </c>
       <c r="D7" s="3">
-        <v>103062</v>
+        <v>106566</v>
       </c>
       <c r="E7" s="3">
-        <v>194796</v>
+        <v>201419</v>
       </c>
       <c r="F7" s="3">
-        <v>284199</v>
+        <v>293862</v>
       </c>
       <c r="G7" s="3">
-        <v>54744</v>
+        <v>56605</v>
       </c>
       <c r="H7" s="3">
-        <v>49269</v>
+        <v>50944</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -650,25 +650,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>58670</v>
+        <v>60665</v>
       </c>
       <c r="C8" s="3">
-        <v>83821</v>
+        <v>86671</v>
       </c>
       <c r="D8" s="3">
-        <v>103027</v>
+        <v>106530</v>
       </c>
       <c r="E8" s="3">
-        <v>196399</v>
+        <v>203077</v>
       </c>
       <c r="F8" s="3">
-        <v>289475</v>
+        <v>299317</v>
       </c>
       <c r="G8" s="3">
-        <v>54482</v>
+        <v>56334</v>
       </c>
       <c r="H8" s="3">
-        <v>50850</v>
+        <v>52579</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -676,25 +676,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>67337</v>
+        <v>69626</v>
       </c>
       <c r="C9" s="3">
-        <v>94884</v>
+        <v>98110</v>
       </c>
       <c r="D9" s="3">
-        <v>118954</v>
+        <v>122998</v>
       </c>
       <c r="E9" s="3">
-        <v>227873</v>
+        <v>235621</v>
       </c>
       <c r="F9" s="3">
-        <v>334245</v>
+        <v>345609</v>
       </c>
       <c r="G9" s="3">
-        <v>63696</v>
+        <v>65862</v>
       </c>
       <c r="H9" s="3">
-        <v>59664</v>
+        <v>61693</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -702,25 +702,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>82066</v>
+        <v>84856</v>
       </c>
       <c r="C10" s="3">
-        <v>115364</v>
+        <v>119286</v>
       </c>
       <c r="D10" s="3">
-        <v>141685</v>
+        <v>146502</v>
       </c>
       <c r="E10" s="3">
-        <v>274345</v>
+        <v>283673</v>
       </c>
       <c r="F10" s="3">
-        <v>391122</v>
+        <v>404420</v>
       </c>
       <c r="G10" s="3">
-        <v>76522</v>
+        <v>79124</v>
       </c>
       <c r="H10" s="3">
-        <v>71679</v>
+        <v>74116</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -728,25 +728,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>75844</v>
+        <v>78423</v>
       </c>
       <c r="C11" s="3">
-        <v>108574</v>
+        <v>112266</v>
       </c>
       <c r="D11" s="3">
-        <v>128202</v>
+        <v>132561</v>
       </c>
       <c r="E11" s="3">
-        <v>217341</v>
+        <v>224731</v>
       </c>
       <c r="F11" s="3">
-        <v>337667</v>
+        <v>349148</v>
       </c>
       <c r="G11" s="3">
-        <v>66057</v>
+        <v>68303</v>
       </c>
       <c r="H11" s="3">
-        <v>56979</v>
+        <v>58916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de precios junio 2025
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -97,6 +97,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -161,7 +162,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -448,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>92263</v>
+        <v>94108</v>
       </c>
       <c r="C2" s="3">
-        <v>132078</v>
+        <v>134720</v>
       </c>
       <c r="D2" s="3">
-        <v>155955</v>
+        <v>159074</v>
       </c>
       <c r="E2" s="3">
-        <v>264389</v>
+        <v>269677</v>
       </c>
       <c r="F2" s="3">
-        <v>410764</v>
+        <v>418979</v>
       </c>
       <c r="G2" s="3">
-        <v>80356</v>
+        <v>81963</v>
       </c>
       <c r="H2" s="3">
-        <v>69313</v>
+        <v>70699</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -520,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>92666</v>
+        <v>94519</v>
       </c>
       <c r="C3" s="3">
-        <v>134110</v>
+        <v>136792</v>
       </c>
       <c r="D3" s="3">
-        <v>157431</v>
+        <v>160580</v>
       </c>
       <c r="E3" s="3">
-        <v>271668</v>
+        <v>277101</v>
       </c>
       <c r="F3" s="3">
-        <v>412036</v>
+        <v>420277</v>
       </c>
       <c r="G3" s="3">
-        <v>80566</v>
+        <v>82177</v>
       </c>
       <c r="H3" s="3">
-        <v>69586</v>
+        <v>70978</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -546,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>104239</v>
+        <v>106324</v>
       </c>
       <c r="C4" s="3">
-        <v>151182</v>
+        <v>154206</v>
       </c>
       <c r="D4" s="3">
-        <v>177395</v>
+        <v>180943</v>
       </c>
       <c r="E4" s="3">
-        <v>305778</v>
+        <v>311894</v>
       </c>
       <c r="F4" s="3">
-        <v>463936</v>
+        <v>473215</v>
       </c>
       <c r="G4" s="3">
-        <v>90538</v>
+        <v>92349</v>
       </c>
       <c r="H4" s="3">
-        <v>78490</v>
+        <v>80060</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -572,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>132423</v>
+        <v>135071</v>
       </c>
       <c r="C5" s="3">
-        <v>189341</v>
+        <v>193128</v>
       </c>
       <c r="D5" s="3">
-        <v>221776</v>
+        <v>226212</v>
       </c>
       <c r="E5" s="3">
-        <v>371643</v>
+        <v>379076</v>
       </c>
       <c r="F5" s="3">
-        <v>553377</v>
+        <v>564445</v>
       </c>
       <c r="G5" s="3">
-        <v>115518</v>
+        <v>117828</v>
       </c>
       <c r="H5" s="3">
-        <v>100478</v>
+        <v>102488</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -598,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>227695</v>
+        <v>232249</v>
       </c>
       <c r="C6" s="3">
-        <v>303301</v>
+        <v>309367</v>
       </c>
       <c r="D6" s="3">
-        <v>399193</v>
+        <v>407177</v>
       </c>
       <c r="E6" s="3">
-        <v>556404</v>
+        <v>567532</v>
       </c>
       <c r="F6" s="3">
-        <v>758227</v>
+        <v>773392</v>
       </c>
       <c r="G6" s="3">
-        <v>199513</v>
+        <v>203503</v>
       </c>
       <c r="H6" s="3">
-        <v>174125</v>
+        <v>177608</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -624,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>59547</v>
+        <v>60738</v>
       </c>
       <c r="C7" s="3">
-        <v>85824</v>
+        <v>87540</v>
       </c>
       <c r="D7" s="3">
-        <v>106566</v>
+        <v>108697</v>
       </c>
       <c r="E7" s="3">
-        <v>201419</v>
+        <v>205447</v>
       </c>
       <c r="F7" s="3">
-        <v>293862</v>
+        <v>299739</v>
       </c>
       <c r="G7" s="3">
-        <v>56605</v>
+        <v>57737</v>
       </c>
       <c r="H7" s="3">
-        <v>50944</v>
+        <v>51963</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -650,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>60665</v>
+        <v>61878</v>
       </c>
       <c r="C8" s="3">
-        <v>86671</v>
+        <v>88404</v>
       </c>
       <c r="D8" s="3">
-        <v>106530</v>
+        <v>108661</v>
       </c>
       <c r="E8" s="3">
-        <v>203077</v>
+        <v>207139</v>
       </c>
       <c r="F8" s="3">
-        <v>299317</v>
+        <v>305303</v>
       </c>
       <c r="G8" s="3">
-        <v>56334</v>
+        <v>57461</v>
       </c>
       <c r="H8" s="3">
-        <v>52579</v>
+        <v>53631</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -676,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>69626</v>
+        <v>71019</v>
       </c>
       <c r="C9" s="3">
-        <v>98110</v>
+        <v>100072</v>
       </c>
       <c r="D9" s="3">
-        <v>122998</v>
+        <v>125458</v>
       </c>
       <c r="E9" s="3">
-        <v>235621</v>
+        <v>240333</v>
       </c>
       <c r="F9" s="3">
-        <v>345609</v>
+        <v>352521</v>
       </c>
       <c r="G9" s="3">
-        <v>65862</v>
+        <v>67179</v>
       </c>
       <c r="H9" s="3">
-        <v>61693</v>
+        <v>62927</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -702,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>84856</v>
+        <v>86553</v>
       </c>
       <c r="C10" s="3">
-        <v>119286</v>
+        <v>121672</v>
       </c>
       <c r="D10" s="3">
-        <v>146502</v>
+        <v>149432</v>
       </c>
       <c r="E10" s="3">
-        <v>283673</v>
+        <v>289346</v>
       </c>
       <c r="F10" s="3">
-        <v>404420</v>
+        <v>412508</v>
       </c>
       <c r="G10" s="3">
-        <v>79124</v>
+        <v>80706</v>
       </c>
       <c r="H10" s="3">
-        <v>74116</v>
+        <v>75598</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -728,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>78423</v>
+        <v>79991</v>
       </c>
       <c r="C11" s="3">
-        <v>112266</v>
+        <v>114511</v>
       </c>
       <c r="D11" s="3">
-        <v>132561</v>
+        <v>135212</v>
       </c>
       <c r="E11" s="3">
-        <v>224731</v>
+        <v>229226</v>
       </c>
       <c r="F11" s="3">
-        <v>349148</v>
+        <v>356131</v>
       </c>
       <c r="G11" s="3">
-        <v>68303</v>
+        <v>69669</v>
       </c>
       <c r="H11" s="3">
-        <v>58916</v>
+        <v>60094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización precios Excel cotizador
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>85968</v>
+        <v>87343</v>
       </c>
       <c r="C2" s="3">
-        <v>116230</v>
+        <v>118090</v>
       </c>
       <c r="D2" s="3">
-        <v>145314</v>
+        <v>147639</v>
       </c>
       <c r="E2" s="3">
-        <v>246350</v>
+        <v>250292</v>
       </c>
       <c r="F2" s="3">
-        <v>425264</v>
+        <v>432068</v>
       </c>
       <c r="G2" s="3">
-        <v>74873</v>
+        <v>76071</v>
       </c>
       <c r="H2" s="3">
-        <v>64584</v>
+        <v>65617</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -521,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>86343</v>
+        <v>87724</v>
       </c>
       <c r="C3" s="3">
-        <v>124959</v>
+        <v>126958</v>
       </c>
       <c r="D3" s="3">
-        <v>146690</v>
+        <v>149037</v>
       </c>
       <c r="E3" s="3">
-        <v>253132</v>
+        <v>257182</v>
       </c>
       <c r="F3" s="3">
-        <v>426581</v>
+        <v>433406</v>
       </c>
       <c r="G3" s="3">
-        <v>75069</v>
+        <v>76270</v>
       </c>
       <c r="H3" s="3">
-        <v>64838</v>
+        <v>65875</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>97127</v>
+        <v>98681</v>
       </c>
       <c r="C4" s="3">
-        <v>125215</v>
+        <v>127218</v>
       </c>
       <c r="D4" s="3">
-        <v>165291</v>
+        <v>167936</v>
       </c>
       <c r="E4" s="3">
-        <v>284915</v>
+        <v>289474</v>
       </c>
       <c r="F4" s="3">
-        <v>480313</v>
+        <v>487998</v>
       </c>
       <c r="G4" s="3">
-        <v>84361</v>
+        <v>85711</v>
       </c>
       <c r="H4" s="3">
-        <v>73135</v>
+        <v>74305</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -573,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>137097</v>
+        <v>139291</v>
       </c>
       <c r="C5" s="3">
-        <v>196025</v>
+        <v>199161</v>
       </c>
       <c r="D5" s="3">
-        <v>229605</v>
+        <v>233279</v>
       </c>
       <c r="E5" s="3">
-        <v>384762</v>
+        <v>390918</v>
       </c>
       <c r="F5" s="3">
-        <v>572912</v>
+        <v>582079</v>
       </c>
       <c r="G5" s="3">
-        <v>119595</v>
+        <v>121509</v>
       </c>
       <c r="H5" s="3">
-        <v>104025</v>
+        <v>105689</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -599,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>235733</v>
+        <v>239505</v>
       </c>
       <c r="C6" s="3">
-        <v>314008</v>
+        <v>319032</v>
       </c>
       <c r="D6" s="3">
-        <v>413285</v>
+        <v>419898</v>
       </c>
       <c r="E6" s="3">
-        <v>576045</v>
+        <v>585262</v>
       </c>
       <c r="F6" s="3">
-        <v>784993</v>
+        <v>797553</v>
       </c>
       <c r="G6" s="3">
-        <v>206556</v>
+        <v>209861</v>
       </c>
       <c r="H6" s="3">
-        <v>180272</v>
+        <v>183156</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -625,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>61649</v>
+        <v>62635</v>
       </c>
       <c r="C7" s="3">
-        <v>88853</v>
+        <v>90275</v>
       </c>
       <c r="D7" s="3">
-        <v>110327</v>
+        <v>112092</v>
       </c>
       <c r="E7" s="3">
-        <v>208529</v>
+        <v>211865</v>
       </c>
       <c r="F7" s="3">
-        <v>304235</v>
+        <v>309103</v>
       </c>
       <c r="G7" s="3">
-        <v>58603</v>
+        <v>59541</v>
       </c>
       <c r="H7" s="3">
-        <v>52742</v>
+        <v>53586</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>62806</v>
+        <v>63811</v>
       </c>
       <c r="C8" s="3">
-        <v>89730</v>
+        <v>91166</v>
       </c>
       <c r="D8" s="3">
-        <v>110291</v>
+        <v>112056</v>
       </c>
       <c r="E8" s="3">
-        <v>210246</v>
+        <v>213610</v>
       </c>
       <c r="F8" s="3">
-        <v>309883</v>
+        <v>314841</v>
       </c>
       <c r="G8" s="3">
-        <v>58323</v>
+        <v>59256</v>
       </c>
       <c r="H8" s="3">
-        <v>54435</v>
+        <v>55306</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>72084</v>
+        <v>73237</v>
       </c>
       <c r="C9" s="3">
-        <v>101573</v>
+        <v>103198</v>
       </c>
       <c r="D9" s="3">
-        <v>127340</v>
+        <v>129377</v>
       </c>
       <c r="E9" s="3">
-        <v>243938</v>
+        <v>247841</v>
       </c>
       <c r="F9" s="3">
-        <v>357809</v>
+        <v>363534</v>
       </c>
       <c r="G9" s="3">
-        <v>68187</v>
+        <v>69278</v>
       </c>
       <c r="H9" s="3">
-        <v>63871</v>
+        <v>64893</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>87851</v>
+        <v>89257</v>
       </c>
       <c r="C10" s="3">
-        <v>123497</v>
+        <v>125473</v>
       </c>
       <c r="D10" s="3">
-        <v>151673</v>
+        <v>154100</v>
       </c>
       <c r="E10" s="3">
-        <v>293686</v>
+        <v>298385</v>
       </c>
       <c r="F10" s="3">
-        <v>418696</v>
+        <v>425395</v>
       </c>
       <c r="G10" s="3">
-        <v>81917</v>
+        <v>83228</v>
       </c>
       <c r="H10" s="3">
-        <v>76732</v>
+        <v>77960</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>73072</v>
+        <v>74241</v>
       </c>
       <c r="C11" s="3">
-        <v>98794</v>
+        <v>100375</v>
       </c>
       <c r="D11" s="3">
-        <v>123516</v>
+        <v>125492</v>
       </c>
       <c r="E11" s="3">
-        <v>209398</v>
+        <v>212748</v>
       </c>
       <c r="F11" s="3">
-        <v>361473</v>
+        <v>367257</v>
       </c>
       <c r="G11" s="3">
-        <v>63643</v>
+        <v>64661</v>
       </c>
       <c r="H11" s="3">
-        <v>54896</v>
+        <v>55774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de lista de precios cotizador.xlsx
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>87343</v>
+        <v>89003</v>
       </c>
       <c r="C2" s="3">
-        <v>118090</v>
+        <v>120334</v>
       </c>
       <c r="D2" s="3">
-        <v>147639</v>
+        <v>150444</v>
       </c>
       <c r="E2" s="3">
-        <v>250292</v>
+        <v>255048</v>
       </c>
       <c r="F2" s="3">
-        <v>432068</v>
+        <v>440277</v>
       </c>
       <c r="G2" s="3">
-        <v>76071</v>
+        <v>77516</v>
       </c>
       <c r="H2" s="3">
-        <v>65617</v>
+        <v>66864</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -521,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>87724</v>
+        <v>89391</v>
       </c>
       <c r="C3" s="3">
-        <v>126958</v>
+        <v>129370</v>
       </c>
       <c r="D3" s="3">
-        <v>149037</v>
+        <v>151869</v>
       </c>
       <c r="E3" s="3">
-        <v>257182</v>
+        <v>262068</v>
       </c>
       <c r="F3" s="3">
-        <v>433406</v>
+        <v>441641</v>
       </c>
       <c r="G3" s="3">
-        <v>76270</v>
+        <v>77719</v>
       </c>
       <c r="H3" s="3">
-        <v>65875</v>
+        <v>67127</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>98681</v>
+        <v>100556</v>
       </c>
       <c r="C4" s="3">
-        <v>127218</v>
+        <v>129635</v>
       </c>
       <c r="D4" s="3">
-        <v>167936</v>
+        <v>171127</v>
       </c>
       <c r="E4" s="3">
-        <v>289474</v>
+        <v>294974</v>
       </c>
       <c r="F4" s="3">
-        <v>487998</v>
+        <v>497270</v>
       </c>
       <c r="G4" s="3">
-        <v>85711</v>
+        <v>87340</v>
       </c>
       <c r="H4" s="3">
-        <v>74305</v>
+        <v>75717</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -573,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>139291</v>
+        <v>141938</v>
       </c>
       <c r="C5" s="3">
-        <v>199161</v>
+        <v>202945</v>
       </c>
       <c r="D5" s="3">
-        <v>233279</v>
+        <v>237711</v>
       </c>
       <c r="E5" s="3">
-        <v>390918</v>
+        <v>398345</v>
       </c>
       <c r="F5" s="3">
-        <v>582079</v>
+        <v>593139</v>
       </c>
       <c r="G5" s="3">
-        <v>121509</v>
+        <v>123818</v>
       </c>
       <c r="H5" s="3">
-        <v>105689</v>
+        <v>107697</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -599,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>239505</v>
+        <v>244056</v>
       </c>
       <c r="C6" s="3">
-        <v>319032</v>
+        <v>325094</v>
       </c>
       <c r="D6" s="3">
-        <v>419898</v>
+        <v>427876</v>
       </c>
       <c r="E6" s="3">
-        <v>585262</v>
+        <v>596382</v>
       </c>
       <c r="F6" s="3">
-        <v>797553</v>
+        <v>812707</v>
       </c>
       <c r="G6" s="3">
-        <v>209861</v>
+        <v>213848</v>
       </c>
       <c r="H6" s="3">
-        <v>183156</v>
+        <v>186636</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -625,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>62635</v>
+        <v>63825</v>
       </c>
       <c r="C7" s="3">
-        <v>90275</v>
+        <v>91990</v>
       </c>
       <c r="D7" s="3">
-        <v>112092</v>
+        <v>114222</v>
       </c>
       <c r="E7" s="3">
-        <v>211865</v>
+        <v>215890</v>
       </c>
       <c r="F7" s="3">
-        <v>309103</v>
+        <v>314976</v>
       </c>
       <c r="G7" s="3">
-        <v>59541</v>
+        <v>60672</v>
       </c>
       <c r="H7" s="3">
-        <v>53586</v>
+        <v>54604</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>63811</v>
+        <v>65023</v>
       </c>
       <c r="C8" s="3">
-        <v>91166</v>
+        <v>92898</v>
       </c>
       <c r="D8" s="3">
-        <v>112056</v>
+        <v>114185</v>
       </c>
       <c r="E8" s="3">
-        <v>213610</v>
+        <v>217669</v>
       </c>
       <c r="F8" s="3">
-        <v>314841</v>
+        <v>320823</v>
       </c>
       <c r="G8" s="3">
-        <v>59256</v>
+        <v>60382</v>
       </c>
       <c r="H8" s="3">
-        <v>55306</v>
+        <v>56357</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>73237</v>
+        <v>74629</v>
       </c>
       <c r="C9" s="3">
-        <v>103198</v>
+        <v>105159</v>
       </c>
       <c r="D9" s="3">
-        <v>129377</v>
+        <v>131835</v>
       </c>
       <c r="E9" s="3">
-        <v>247841</v>
+        <v>252550</v>
       </c>
       <c r="F9" s="3">
-        <v>363534</v>
+        <v>370441</v>
       </c>
       <c r="G9" s="3">
-        <v>69278</v>
+        <v>70594</v>
       </c>
       <c r="H9" s="3">
-        <v>64893</v>
+        <v>66126</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>89257</v>
+        <v>90953</v>
       </c>
       <c r="C10" s="3">
-        <v>125473</v>
+        <v>127857</v>
       </c>
       <c r="D10" s="3">
-        <v>154100</v>
+        <v>157028</v>
       </c>
       <c r="E10" s="3">
-        <v>298385</v>
+        <v>304054</v>
       </c>
       <c r="F10" s="3">
-        <v>425395</v>
+        <v>433478</v>
       </c>
       <c r="G10" s="3">
-        <v>83228</v>
+        <v>84809</v>
       </c>
       <c r="H10" s="3">
-        <v>77960</v>
+        <v>79441</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>74241</v>
+        <v>75652</v>
       </c>
       <c r="C11" s="3">
-        <v>100375</v>
+        <v>102282</v>
       </c>
       <c r="D11" s="3">
-        <v>125492</v>
+        <v>127876</v>
       </c>
       <c r="E11" s="3">
-        <v>212748</v>
+        <v>216790</v>
       </c>
       <c r="F11" s="3">
-        <v>367257</v>
+        <v>374235</v>
       </c>
       <c r="G11" s="3">
-        <v>64661</v>
+        <v>65890</v>
       </c>
       <c r="H11" s="3">
-        <v>55774</v>
+        <v>56834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de lista de precios cotizador.xlsx (Octubre 2025)
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>89003</v>
+        <v>90739</v>
       </c>
       <c r="C2" s="3">
-        <v>120334</v>
+        <v>122681</v>
       </c>
       <c r="D2" s="3">
-        <v>150444</v>
+        <v>153378</v>
       </c>
       <c r="E2" s="3">
-        <v>255048</v>
+        <v>260021</v>
       </c>
       <c r="F2" s="3">
-        <v>440277</v>
+        <v>448862</v>
       </c>
       <c r="G2" s="3">
-        <v>77516</v>
+        <v>79028</v>
       </c>
       <c r="H2" s="3">
-        <v>66864</v>
+        <v>68168</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -521,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>89391</v>
+        <v>91134</v>
       </c>
       <c r="C3" s="3">
-        <v>129370</v>
+        <v>131893</v>
       </c>
       <c r="D3" s="3">
-        <v>151869</v>
+        <v>154830</v>
       </c>
       <c r="E3" s="3">
-        <v>262068</v>
+        <v>267178</v>
       </c>
       <c r="F3" s="3">
-        <v>441641</v>
+        <v>450253</v>
       </c>
       <c r="G3" s="3">
-        <v>77719</v>
+        <v>79235</v>
       </c>
       <c r="H3" s="3">
-        <v>67127</v>
+        <v>68436</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>100556</v>
+        <v>102517</v>
       </c>
       <c r="C4" s="3">
-        <v>129635</v>
+        <v>132163</v>
       </c>
       <c r="D4" s="3">
-        <v>171127</v>
+        <v>174464</v>
       </c>
       <c r="E4" s="3">
-        <v>294974</v>
+        <v>300726</v>
       </c>
       <c r="F4" s="3">
-        <v>497270</v>
+        <v>506967</v>
       </c>
       <c r="G4" s="3">
-        <v>87340</v>
+        <v>89043</v>
       </c>
       <c r="H4" s="3">
-        <v>75717</v>
+        <v>77193</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -573,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>141938</v>
+        <v>144706</v>
       </c>
       <c r="C5" s="3">
-        <v>202945</v>
+        <v>206902</v>
       </c>
       <c r="D5" s="3">
-        <v>237711</v>
+        <v>242346</v>
       </c>
       <c r="E5" s="3">
-        <v>398345</v>
+        <v>406113</v>
       </c>
       <c r="F5" s="3">
-        <v>593139</v>
+        <v>604705</v>
       </c>
       <c r="G5" s="3">
-        <v>123818</v>
+        <v>126232</v>
       </c>
       <c r="H5" s="3">
-        <v>107697</v>
+        <v>109797</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -599,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>244056</v>
+        <v>248815</v>
       </c>
       <c r="C6" s="3">
-        <v>325094</v>
+        <v>331433</v>
       </c>
       <c r="D6" s="3">
-        <v>427876</v>
+        <v>436220</v>
       </c>
       <c r="E6" s="3">
-        <v>596382</v>
+        <v>608011</v>
       </c>
       <c r="F6" s="3">
-        <v>812707</v>
+        <v>828555</v>
       </c>
       <c r="G6" s="3">
-        <v>213848</v>
+        <v>218018</v>
       </c>
       <c r="H6" s="3">
-        <v>186636</v>
+        <v>190275</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -625,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>63825</v>
+        <v>65070</v>
       </c>
       <c r="C7" s="3">
-        <v>91990</v>
+        <v>93784</v>
       </c>
       <c r="D7" s="3">
-        <v>114222</v>
+        <v>116449</v>
       </c>
       <c r="E7" s="3">
-        <v>215890</v>
+        <v>220100</v>
       </c>
       <c r="F7" s="3">
-        <v>314976</v>
+        <v>321118</v>
       </c>
       <c r="G7" s="3">
-        <v>60672</v>
+        <v>61855</v>
       </c>
       <c r="H7" s="3">
-        <v>54604</v>
+        <v>55669</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>65023</v>
+        <v>66291</v>
       </c>
       <c r="C8" s="3">
-        <v>92898</v>
+        <v>94710</v>
       </c>
       <c r="D8" s="3">
-        <v>114185</v>
+        <v>116412</v>
       </c>
       <c r="E8" s="3">
-        <v>217669</v>
+        <v>221914</v>
       </c>
       <c r="F8" s="3">
-        <v>320823</v>
+        <v>327079</v>
       </c>
       <c r="G8" s="3">
-        <v>60382</v>
+        <v>61559</v>
       </c>
       <c r="H8" s="3">
-        <v>56357</v>
+        <v>57456</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>74629</v>
+        <v>76084</v>
       </c>
       <c r="C9" s="3">
-        <v>105159</v>
+        <v>107210</v>
       </c>
       <c r="D9" s="3">
-        <v>131835</v>
+        <v>134406</v>
       </c>
       <c r="E9" s="3">
-        <v>252550</v>
+        <v>257475</v>
       </c>
       <c r="F9" s="3">
-        <v>370441</v>
+        <v>377665</v>
       </c>
       <c r="G9" s="3">
-        <v>70594</v>
+        <v>71971</v>
       </c>
       <c r="H9" s="3">
-        <v>66126</v>
+        <v>67415</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>90953</v>
+        <v>92727</v>
       </c>
       <c r="C10" s="3">
-        <v>127857</v>
+        <v>130350</v>
       </c>
       <c r="D10" s="3">
-        <v>157028</v>
+        <v>160090</v>
       </c>
       <c r="E10" s="3">
-        <v>304054</v>
+        <v>309983</v>
       </c>
       <c r="F10" s="3">
-        <v>433478</v>
+        <v>441931</v>
       </c>
       <c r="G10" s="3">
-        <v>84809</v>
+        <v>86463</v>
       </c>
       <c r="H10" s="3">
-        <v>79441</v>
+        <v>80990</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>75652</v>
+        <v>77127</v>
       </c>
       <c r="C11" s="3">
-        <v>102282</v>
+        <v>104276</v>
       </c>
       <c r="D11" s="3">
-        <v>127876</v>
+        <v>130370</v>
       </c>
       <c r="E11" s="3">
-        <v>216790</v>
+        <v>221017</v>
       </c>
       <c r="F11" s="3">
-        <v>374235</v>
+        <v>381533</v>
       </c>
       <c r="G11" s="3">
-        <v>65890</v>
+        <v>67175</v>
       </c>
       <c r="H11" s="3">
-        <v>56834</v>
+        <v>57942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de lista de precios cotizador.xlsx (Noviembre 2025)
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I19" sqref="I19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>90739</v>
+        <v>92690</v>
       </c>
       <c r="C2" s="3">
-        <v>122681</v>
+        <v>119053</v>
       </c>
       <c r="D2" s="3">
-        <v>153378</v>
+        <v>156676</v>
       </c>
       <c r="E2" s="3">
-        <v>260021</v>
+        <v>265611</v>
       </c>
       <c r="F2" s="3">
-        <v>448862</v>
+        <v>458513</v>
       </c>
       <c r="G2" s="3">
-        <v>79028</v>
+        <v>80727</v>
       </c>
       <c r="H2" s="3">
-        <v>68168</v>
+        <v>69634</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -521,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>91134</v>
+        <v>93093</v>
       </c>
       <c r="C3" s="3">
-        <v>131893</v>
+        <v>127992</v>
       </c>
       <c r="D3" s="3">
-        <v>154830</v>
+        <v>158159</v>
       </c>
       <c r="E3" s="3">
-        <v>267178</v>
+        <v>272922</v>
       </c>
       <c r="F3" s="3">
-        <v>450253</v>
+        <v>459933</v>
       </c>
       <c r="G3" s="3">
-        <v>79235</v>
+        <v>80939</v>
       </c>
       <c r="H3" s="3">
-        <v>68436</v>
+        <v>69907</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>102517</v>
+        <v>104721</v>
       </c>
       <c r="C4" s="3">
-        <v>132163</v>
+        <v>128254</v>
       </c>
       <c r="D4" s="3">
-        <v>174464</v>
+        <v>178215</v>
       </c>
       <c r="E4" s="3">
-        <v>300726</v>
+        <v>307192</v>
       </c>
       <c r="F4" s="3">
-        <v>506967</v>
+        <v>517867</v>
       </c>
       <c r="G4" s="3">
-        <v>89043</v>
+        <v>90957</v>
       </c>
       <c r="H4" s="3">
-        <v>77193</v>
+        <v>78853</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -573,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>144706</v>
+        <v>147817</v>
       </c>
       <c r="C5" s="3">
-        <v>206902</v>
+        <v>211350</v>
       </c>
       <c r="D5" s="3">
-        <v>242346</v>
+        <v>247556</v>
       </c>
       <c r="E5" s="3">
-        <v>406113</v>
+        <v>414844</v>
       </c>
       <c r="F5" s="3">
-        <v>604705</v>
+        <v>617706</v>
       </c>
       <c r="G5" s="3">
-        <v>126232</v>
+        <v>128946</v>
       </c>
       <c r="H5" s="3">
-        <v>109797</v>
+        <v>112158</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -599,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>248815</v>
+        <v>254165</v>
       </c>
       <c r="C6" s="3">
-        <v>331433</v>
+        <v>338559</v>
       </c>
       <c r="D6" s="3">
-        <v>436220</v>
+        <v>445599</v>
       </c>
       <c r="E6" s="3">
-        <v>608011</v>
+        <v>621083</v>
       </c>
       <c r="F6" s="3">
-        <v>828555</v>
+        <v>846369</v>
       </c>
       <c r="G6" s="3">
-        <v>218018</v>
+        <v>222705</v>
       </c>
       <c r="H6" s="3">
-        <v>190275</v>
+        <v>194366</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -625,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>65070</v>
+        <v>66469</v>
       </c>
       <c r="C7" s="3">
-        <v>93784</v>
+        <v>91010</v>
       </c>
       <c r="D7" s="3">
-        <v>116449</v>
+        <v>118953</v>
       </c>
       <c r="E7" s="3">
-        <v>220100</v>
+        <v>224832</v>
       </c>
       <c r="F7" s="3">
-        <v>321118</v>
+        <v>328022</v>
       </c>
       <c r="G7" s="3">
-        <v>61855</v>
+        <v>63185</v>
       </c>
       <c r="H7" s="3">
-        <v>55669</v>
+        <v>56866</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>66291</v>
+        <v>67716</v>
       </c>
       <c r="C8" s="3">
-        <v>94710</v>
+        <v>91909</v>
       </c>
       <c r="D8" s="3">
-        <v>116412</v>
+        <v>118915</v>
       </c>
       <c r="E8" s="3">
-        <v>221914</v>
+        <v>226685</v>
       </c>
       <c r="F8" s="3">
-        <v>327079</v>
+        <v>334111</v>
       </c>
       <c r="G8" s="3">
-        <v>61559</v>
+        <v>62883</v>
       </c>
       <c r="H8" s="3">
-        <v>57456</v>
+        <v>58691</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>76084</v>
+        <v>77720</v>
       </c>
       <c r="C9" s="3">
-        <v>107210</v>
+        <v>104039</v>
       </c>
       <c r="D9" s="3">
-        <v>134406</v>
+        <v>137296</v>
       </c>
       <c r="E9" s="3">
-        <v>257475</v>
+        <v>263011</v>
       </c>
       <c r="F9" s="3">
-        <v>377665</v>
+        <v>385785</v>
       </c>
       <c r="G9" s="3">
-        <v>71971</v>
+        <v>73518</v>
       </c>
       <c r="H9" s="3">
-        <v>67415</v>
+        <v>68864</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>92727</v>
+        <v>94721</v>
       </c>
       <c r="C10" s="3">
-        <v>130350</v>
+        <v>133153</v>
       </c>
       <c r="D10" s="3">
-        <v>160090</v>
+        <v>163532</v>
       </c>
       <c r="E10" s="3">
-        <v>309983</v>
+        <v>316648</v>
       </c>
       <c r="F10" s="3">
-        <v>441931</v>
+        <v>451433</v>
       </c>
       <c r="G10" s="3">
-        <v>86463</v>
+        <v>88322</v>
       </c>
       <c r="H10" s="3">
-        <v>80990</v>
+        <v>82731</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>77127</v>
+        <v>78785</v>
       </c>
       <c r="C11" s="3">
-        <v>104276</v>
+        <v>101192</v>
       </c>
       <c r="D11" s="3">
-        <v>130370</v>
+        <v>133173</v>
       </c>
       <c r="E11" s="3">
-        <v>221017</v>
+        <v>225769</v>
       </c>
       <c r="F11" s="3">
-        <v>381533</v>
+        <v>389736</v>
       </c>
       <c r="G11" s="3">
-        <v>67175</v>
+        <v>68619</v>
       </c>
       <c r="H11" s="3">
-        <v>57942</v>
+        <v>59188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de precios cotizador - diciembre 2025
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:J19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>92690</v>
+        <v>94868</v>
       </c>
       <c r="C2" s="3">
-        <v>119053</v>
+        <v>121851</v>
       </c>
       <c r="D2" s="3">
-        <v>156676</v>
+        <v>160358</v>
       </c>
       <c r="E2" s="3">
-        <v>265611</v>
+        <v>271853</v>
       </c>
       <c r="F2" s="3">
-        <v>458513</v>
+        <v>469288</v>
       </c>
       <c r="G2" s="3">
-        <v>80727</v>
+        <v>82624</v>
       </c>
       <c r="H2" s="3">
-        <v>69634</v>
+        <v>71270</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -521,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>93093</v>
+        <v>95281</v>
       </c>
       <c r="C3" s="3">
-        <v>127992</v>
+        <v>131000</v>
       </c>
       <c r="D3" s="3">
-        <v>158159</v>
+        <v>161876</v>
       </c>
       <c r="E3" s="3">
-        <v>272922</v>
+        <v>279336</v>
       </c>
       <c r="F3" s="3">
-        <v>459933</v>
+        <v>470741</v>
       </c>
       <c r="G3" s="3">
-        <v>80939</v>
+        <v>82841</v>
       </c>
       <c r="H3" s="3">
-        <v>69907</v>
+        <v>71550</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>104721</v>
+        <v>107182</v>
       </c>
       <c r="C4" s="3">
-        <v>128254</v>
+        <v>131268</v>
       </c>
       <c r="D4" s="3">
-        <v>178215</v>
+        <v>182403</v>
       </c>
       <c r="E4" s="3">
-        <v>307192</v>
+        <v>314411</v>
       </c>
       <c r="F4" s="3">
-        <v>517867</v>
+        <v>530037</v>
       </c>
       <c r="G4" s="3">
-        <v>90957</v>
+        <v>93094</v>
       </c>
       <c r="H4" s="3">
-        <v>78853</v>
+        <v>80706</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -573,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>147817</v>
+        <v>151291</v>
       </c>
       <c r="C5" s="3">
-        <v>211350</v>
+        <v>216317</v>
       </c>
       <c r="D5" s="3">
-        <v>247556</v>
+        <v>253374</v>
       </c>
       <c r="E5" s="3">
-        <v>414844</v>
+        <v>424593</v>
       </c>
       <c r="F5" s="3">
-        <v>617706</v>
+        <v>632222</v>
       </c>
       <c r="G5" s="3">
-        <v>128946</v>
+        <v>131976</v>
       </c>
       <c r="H5" s="3">
-        <v>112158</v>
+        <v>114794</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -599,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>254165</v>
+        <v>260138</v>
       </c>
       <c r="C6" s="3">
-        <v>338559</v>
+        <v>346515</v>
       </c>
       <c r="D6" s="3">
-        <v>445599</v>
+        <v>456071</v>
       </c>
       <c r="E6" s="3">
-        <v>621083</v>
+        <v>635678</v>
       </c>
       <c r="F6" s="3">
-        <v>846369</v>
+        <v>866259</v>
       </c>
       <c r="G6" s="3">
-        <v>222705</v>
+        <v>227939</v>
       </c>
       <c r="H6" s="3">
-        <v>194366</v>
+        <v>198934</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -625,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>66469</v>
+        <v>68031</v>
       </c>
       <c r="C7" s="3">
-        <v>91010</v>
+        <v>93149</v>
       </c>
       <c r="D7" s="3">
-        <v>118953</v>
+        <v>121748</v>
       </c>
       <c r="E7" s="3">
-        <v>224832</v>
+        <v>230116</v>
       </c>
       <c r="F7" s="3">
-        <v>328022</v>
+        <v>335731</v>
       </c>
       <c r="G7" s="3">
-        <v>63185</v>
+        <v>64670</v>
       </c>
       <c r="H7" s="3">
-        <v>56866</v>
+        <v>58202</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>67716</v>
+        <v>69307</v>
       </c>
       <c r="C8" s="3">
-        <v>91909</v>
+        <v>94069</v>
       </c>
       <c r="D8" s="3">
-        <v>118915</v>
+        <v>121710</v>
       </c>
       <c r="E8" s="3">
-        <v>226685</v>
+        <v>232012</v>
       </c>
       <c r="F8" s="3">
-        <v>334111</v>
+        <v>341963</v>
       </c>
       <c r="G8" s="3">
-        <v>62883</v>
+        <v>64361</v>
       </c>
       <c r="H8" s="3">
-        <v>58691</v>
+        <v>60070</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>77720</v>
+        <v>79546</v>
       </c>
       <c r="C9" s="3">
-        <v>104039</v>
+        <v>106484</v>
       </c>
       <c r="D9" s="3">
-        <v>137296</v>
+        <v>140522</v>
       </c>
       <c r="E9" s="3">
-        <v>263011</v>
+        <v>269192</v>
       </c>
       <c r="F9" s="3">
-        <v>385785</v>
+        <v>394851</v>
       </c>
       <c r="G9" s="3">
-        <v>73518</v>
+        <v>75246</v>
       </c>
       <c r="H9" s="3">
-        <v>68864</v>
+        <v>70482</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>94721</v>
+        <v>96947</v>
       </c>
       <c r="C10" s="3">
-        <v>133153</v>
+        <v>136282</v>
       </c>
       <c r="D10" s="3">
-        <v>163532</v>
+        <v>167375</v>
       </c>
       <c r="E10" s="3">
-        <v>316648</v>
+        <v>324089</v>
       </c>
       <c r="F10" s="3">
-        <v>451433</v>
+        <v>462042</v>
       </c>
       <c r="G10" s="3">
-        <v>88322</v>
+        <v>90398</v>
       </c>
       <c r="H10" s="3">
-        <v>82731</v>
+        <v>84675</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>78785</v>
+        <v>80636</v>
       </c>
       <c r="C11" s="3">
-        <v>101192</v>
+        <v>103570</v>
       </c>
       <c r="D11" s="3">
-        <v>133173</v>
+        <v>136303</v>
       </c>
       <c r="E11" s="3">
-        <v>225769</v>
+        <v>231075</v>
       </c>
       <c r="F11" s="3">
-        <v>389736</v>
+        <v>398895</v>
       </c>
       <c r="G11" s="3">
-        <v>68619</v>
+        <v>70232</v>
       </c>
       <c r="H11" s="3">
-        <v>59188</v>
+        <v>60579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update price tables - Ene 2026
</commit_message>
<xml_diff>
--- a/cotizador.xlsx
+++ b/cotizador.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +495,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>94868</v>
+        <v>97287</v>
       </c>
       <c r="C2" s="3">
-        <v>121851</v>
+        <v>124958</v>
       </c>
       <c r="D2" s="3">
-        <v>160358</v>
+        <v>164447</v>
       </c>
       <c r="E2" s="3">
-        <v>271853</v>
+        <v>278785</v>
       </c>
       <c r="F2" s="3">
-        <v>469288</v>
+        <v>481255</v>
       </c>
       <c r="G2" s="3">
-        <v>82624</v>
+        <v>84731</v>
       </c>
       <c r="H2" s="3">
-        <v>71270</v>
+        <v>73087</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -521,25 +521,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>95281</v>
+        <v>97711</v>
       </c>
       <c r="C3" s="3">
-        <v>131000</v>
+        <v>134341</v>
       </c>
       <c r="D3" s="3">
-        <v>161876</v>
+        <v>166004</v>
       </c>
       <c r="E3" s="3">
-        <v>279336</v>
+        <v>286459</v>
       </c>
       <c r="F3" s="3">
-        <v>470741</v>
+        <v>482745</v>
       </c>
       <c r="G3" s="3">
-        <v>82841</v>
+        <v>84953</v>
       </c>
       <c r="H3" s="3">
-        <v>71550</v>
+        <v>73375</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>107182</v>
+        <v>109915</v>
       </c>
       <c r="C4" s="3">
-        <v>131268</v>
+        <v>134615</v>
       </c>
       <c r="D4" s="3">
-        <v>182403</v>
+        <v>187054</v>
       </c>
       <c r="E4" s="3">
-        <v>314411</v>
+        <v>322428</v>
       </c>
       <c r="F4" s="3">
-        <v>530037</v>
+        <v>543553</v>
       </c>
       <c r="G4" s="3">
-        <v>93094</v>
+        <v>95468</v>
       </c>
       <c r="H4" s="3">
-        <v>80706</v>
+        <v>82764</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -573,25 +573,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>151291</v>
+        <v>155149</v>
       </c>
       <c r="C5" s="3">
-        <v>216317</v>
+        <v>221833</v>
       </c>
       <c r="D5" s="3">
-        <v>253374</v>
+        <v>259835</v>
       </c>
       <c r="E5" s="3">
-        <v>424593</v>
+        <v>435420</v>
       </c>
       <c r="F5" s="3">
-        <v>632222</v>
+        <v>648344</v>
       </c>
       <c r="G5" s="3">
-        <v>131976</v>
+        <v>135341</v>
       </c>
       <c r="H5" s="3">
-        <v>114794</v>
+        <v>117721</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -599,25 +599,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>260138</v>
+        <v>266772</v>
       </c>
       <c r="C6" s="3">
-        <v>346515</v>
+        <v>355351</v>
       </c>
       <c r="D6" s="3">
-        <v>456071</v>
+        <v>467701</v>
       </c>
       <c r="E6" s="3">
-        <v>635678</v>
+        <v>651888</v>
       </c>
       <c r="F6" s="3">
-        <v>866259</v>
+        <v>888349</v>
       </c>
       <c r="G6" s="3">
-        <v>227939</v>
+        <v>233751</v>
       </c>
       <c r="H6" s="3">
-        <v>198934</v>
+        <v>204007</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -625,25 +625,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>68031</v>
+        <v>69766</v>
       </c>
       <c r="C7" s="3">
-        <v>93149</v>
+        <v>95524</v>
       </c>
       <c r="D7" s="3">
-        <v>121748</v>
+        <v>124853</v>
       </c>
       <c r="E7" s="3">
-        <v>230116</v>
+        <v>235984</v>
       </c>
       <c r="F7" s="3">
-        <v>335731</v>
+        <v>344292</v>
       </c>
       <c r="G7" s="3">
-        <v>64670</v>
+        <v>66319</v>
       </c>
       <c r="H7" s="3">
-        <v>58202</v>
+        <v>59686</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,25 +651,25 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>69307</v>
+        <v>71074</v>
       </c>
       <c r="C8" s="3">
-        <v>94069</v>
+        <v>96468</v>
       </c>
       <c r="D8" s="3">
-        <v>121710</v>
+        <v>124814</v>
       </c>
       <c r="E8" s="3">
-        <v>232012</v>
+        <v>237928</v>
       </c>
       <c r="F8" s="3">
-        <v>341963</v>
+        <v>350683</v>
       </c>
       <c r="G8" s="3">
-        <v>64361</v>
+        <v>66002</v>
       </c>
       <c r="H8" s="3">
-        <v>60070</v>
+        <v>61602</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -677,25 +677,25 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>79546</v>
+        <v>81574</v>
       </c>
       <c r="C9" s="3">
-        <v>106484</v>
+        <v>109199</v>
       </c>
       <c r="D9" s="3">
-        <v>140522</v>
+        <v>144105</v>
       </c>
       <c r="E9" s="3">
-        <v>269192</v>
+        <v>276056</v>
       </c>
       <c r="F9" s="3">
-        <v>394851</v>
+        <v>404920</v>
       </c>
       <c r="G9" s="3">
-        <v>75246</v>
+        <v>77165</v>
       </c>
       <c r="H9" s="3">
-        <v>70482</v>
+        <v>72279</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,25 +703,25 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>96947</v>
+        <v>99419</v>
       </c>
       <c r="C10" s="3">
-        <v>136282</v>
+        <v>139757</v>
       </c>
       <c r="D10" s="3">
-        <v>167375</v>
+        <v>171643</v>
       </c>
       <c r="E10" s="3">
-        <v>324089</v>
+        <v>332353</v>
       </c>
       <c r="F10" s="3">
-        <v>462042</v>
+        <v>473824</v>
       </c>
       <c r="G10" s="3">
-        <v>90398</v>
+        <v>92703</v>
       </c>
       <c r="H10" s="3">
-        <v>84675</v>
+        <v>86834</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,25 +729,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>80636</v>
+        <v>82692</v>
       </c>
       <c r="C11" s="3">
-        <v>103570</v>
+        <v>106211</v>
       </c>
       <c r="D11" s="3">
-        <v>136303</v>
+        <v>139779</v>
       </c>
       <c r="E11" s="3">
-        <v>231075</v>
+        <v>236967</v>
       </c>
       <c r="F11" s="3">
-        <v>398895</v>
+        <v>409067</v>
       </c>
       <c r="G11" s="3">
-        <v>70232</v>
+        <v>72023</v>
       </c>
       <c r="H11" s="3">
-        <v>60579</v>
+        <v>62124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>